<commit_message>
added data tables: survey1, most_common_apps, speakers_local
</commit_message>
<xml_diff>
--- a/tables/Power_app_criteria.xlsx
+++ b/tables/Power_app_criteria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KAlstad\Documents\Github_C\e-device2\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DE1F6A-EF92-4EE9-89E5-D7607D077E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABF5E51-FCC2-4CC1-96C8-6D4C461925D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33120" yWindow="-19260" windowWidth="24345" windowHeight="15600" activeTab="3" xr2:uid="{E4A5BE10-DBB8-481B-874B-1BDF43DE8625}"/>
+    <workbookView xWindow="28995" yWindow="-19200" windowWidth="24945" windowHeight="15600" activeTab="2" xr2:uid="{E4A5BE10-DBB8-481B-874B-1BDF43DE8625}"/>
   </bookViews>
   <sheets>
     <sheet name="Forms_Options" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="139">
   <si>
     <t>Feature</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>Multi-photo per element (and # limit)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drawing/Annotating on photo </t>
   </si>
   <si>
     <t>Desktop/laptop</t>
@@ -240,9 +237,6 @@
     <t>Price (Option 1)</t>
   </si>
   <si>
-    <t>Price (Option 2)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Business model </t>
   </si>
   <si>
@@ -471,20 +465,9 @@
     <t>Choice lists can entered manually or can be read in from an external file located on the OneDrive or can be a table in an SQL db</t>
   </si>
   <si>
-    <t>Power Apps makes use of the FX coding language which uses Excel type functions, including an "if" function which provides conditional logic for guiding answer series based on responses entered.   If logic accomonateds nested condition questions.</t>
-  </si>
-  <si>
-    <t>Power Apps includes Versions within the Details of an app.  Each Power Apps has a release number; each version update can be annotated with comments; Version of an app must be 'Published' for users to access and use; Note: can only restore apps that have been created within the last 6-months  - so maintaining older versions requires re-saving.</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t xml:space="preserve">Power Apps provides different tools for viewing data that is entered: A gallery is a control that contains other controls and shows a set of data.  A "gallery" is a customizable view of the records which allows for conditional formating (colors for specific values..etc), galleries allow for images and non-text controls (e.g., buttons) to be included in the listing.  
-A data table shows a set of data in a tabular format. "Data tables" are a quick data viewing tool that shows records without any configuration; column order can be easilly changed and filtered.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Using the gallery tool in Power Apps, a user can creat an editible (Excel-like) data grid that can allow a new record to be added or changes or deletions made to existing records.  Function called "Patch" can be build into each field of the editable grid in order to push edits to save dataset.  Alternatively (and more efficiently), all changes can be pushed at once with a Patch query that lists all of the columns that may be changed. </t>
   </si>
   <si>
@@ -498,9 +481,6 @@
   </si>
   <si>
     <t>Constrained choices from an external table or set of rules</t>
-  </si>
-  <si>
-    <t>See above. If commange can be combined with range checks, minimum field submission checks, check for the format of responses.  Error messages can be linked to field checks.  The validity of a series of fields one a form can be check using Form1.Valid command which could be linked to the submit button preventing users from submitting if data validataion fails.</t>
   </si>
   <si>
     <t>The gallery tool allows for a single data table to be split across tabs base on logical nested structure of the data collection.  
@@ -547,24 +527,12 @@
     <t>As many apps as needed</t>
   </si>
   <si>
-    <t>Pay-as-you-go Premium License</t>
-  </si>
-  <si>
-    <t>$10/Active User/Month</t>
-  </si>
-  <si>
     <t>Huge Company</t>
   </si>
   <si>
     <t>Good when use is unpredictable, just starting, not used often.  Connect through Azure account.</t>
   </si>
   <si>
-    <t xml:space="preserve">Per App Premium License </t>
-  </si>
-  <si>
-    <t>Per User Premium License</t>
-  </si>
-  <si>
     <t xml:space="preserve">Power Apps Canvas apps use 'Connections' to to a variety of data sources including Onedrive, Sharepoint, SQL Server; </t>
   </si>
   <si>
@@ -622,36 +590,18 @@
     <t>The PowerApps Component Framework can only be used on Windows. https://learn.microsoft.com/en-us/power-platform/admin/managed-environment-overview</t>
   </si>
   <si>
-    <t>Yes, but some features will not work.</t>
-  </si>
-  <si>
     <t>The Bay Study demonstration app was run/tested on an iphone.</t>
   </si>
   <si>
     <t>The Bay Study demonstration app was run/tested on an Windows 10 system.</t>
   </si>
   <si>
-    <t>“Power Apps per user plan for Government”</t>
-  </si>
-  <si>
     <t>In the Bay Study Power Apps demo, a photo button provides the option to upload a photo or document or take a photo using the camera on the device.</t>
   </si>
   <si>
     <t>Other demos show attachments uploaded to a Power Apps form and added to a Sharepoint list without the use of Power Automate.</t>
   </si>
   <si>
-    <t>Yes;Power Apps has a Camera control function; for a Power App form in Canvas, multiple photos can be linked to a record without the use of a Power Automate routine. https://learn.microsoft.com/en-us/power-apps/maker/canvas-apps/controls/control-add-picture</t>
-  </si>
-  <si>
-    <t>No; Power Apps has a Pen Input control that supports drawing a sketch which can be added as an attachment; but does not have the ability to annotate a picture (to our best knowledge)</t>
-  </si>
-  <si>
-    <t>$20/User/Month</t>
-  </si>
-  <si>
-    <t>$5/App/User/Month</t>
-  </si>
-  <si>
     <t>The Power Platform service is governed by the Microsoft Online Services Terms and the Microsoft Enterprise Privacy Statement</t>
   </si>
   <si>
@@ -661,10 +611,6 @@
     <t>Power Apps for Government Plans</t>
   </si>
   <si>
-    <t>The Power Apps per User plan for Government (App Developer Licents) is About $17/Month; 
-The End-User licenses are called The Power Apps per App plan for Government (App User Licence) is about $10/yr each.</t>
-  </si>
-  <si>
     <t>Not easy to get direct technical support; However, lots of resources on the web.</t>
   </si>
   <si>
@@ -680,7 +626,49 @@
     <t>See above link</t>
   </si>
   <si>
-    <t>International (Microsoft was founded on April 4, 1975, by Bill Gates and Paul Allen in Albuquerque, New Mexico.)</t>
+    <t xml:space="preserve">Power Apps makes use of the FX coding language which uses Excel type functions, including an "if" function which provides conditional logic for guiding answer series based on responses entered.  </t>
+  </si>
+  <si>
+    <t>See above. The "If" function can be combined with range checks, minimum field submission checks, check for the format of responses.  Error messages can be linked to these conditional field checks.  The validity of a series of fields on a form can be checked using Form1.Valid command which could be linked to the submit button preventing users from submitting if data validataion fails.</t>
+  </si>
+  <si>
+    <t>Power Apps includes Versions within the Details of an app.  Each Power Apps app has a release number; each version update can be annotated with comments; Each version of an app must be 'Published' for users to access and use and to generate a unique release number; Note: can only restore apps that have been created within the last 6-months  - so maintaining older versions requires re-saving.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Apps provides different tools for viewing data that is collected: A "gallery" is a control that contains other controls and shows a set of data.  The gallery view is customizable and allows for conditional formating (colors for specific values..etc); galleries allow for images and non-text controls (e.g., buttons) to be included in the listing.  
+A data table shows a set of data in a tabular format. "Data tables" are a quick data viewing tool that shows records without any configuration; column order and column subsets can be easilly changed and filtered.
+</t>
+  </si>
+  <si>
+    <t>International Company</t>
+  </si>
+  <si>
+    <t>Pay-as-you-go Premium License (non- Gov't)</t>
+  </si>
+  <si>
+    <t>Per User Premium License (non-Gov't)</t>
+  </si>
+  <si>
+    <t>The 'Power Apps per User Premium Plan for Government' is an app developer license which is ~ $17/month; 
+The 'Power Apps per App Plan for Government' is the end-user license which is initiated when an app is shared with a new user; this license is ~$10/month for each user</t>
+  </si>
+  <si>
+    <t>$10/Active User/month</t>
+  </si>
+  <si>
+    <t>$20/User/month</t>
+  </si>
+  <si>
+    <t>Yes, but some features ("Components") of form building will not work.</t>
+  </si>
+  <si>
+    <t>;Power Apps has a Camera control function; for a Power App form in Canvas, multiple photos can be linked to a record without the use of a Power Automate routine. https://learn.microsoft.com/en-us/power-apps/maker/canvas-apps/controls/control-add-picture</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Power Apps has a Pen Input control that supports drawing a sketch which can be added as an attachment; but does not have the ability to annotate a picture (to our best knowledge)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drawing-on/ Annotating photo </t>
   </si>
 </sst>
 </file>
@@ -821,7 +809,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -878,18 +866,11 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1213,13 +1194,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FEDC525-B77D-4397-8B91-1C5526620A5B}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="105" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A10" zoomScale="105" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="20" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="3" width="32" style="1" customWidth="1"/>
     <col min="4" max="4" width="47.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="46.42578125" style="1" customWidth="1"/>
@@ -1228,260 +1209,260 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>31</v>
+      <c r="A1" t="s">
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>32</v>
+      <c r="A2" t="s">
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>32</v>
+    </row>
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="F4"/>
     </row>
     <row r="5" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>76</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="212.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>32</v>
+      <c r="A7" t="s">
+        <v>31</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>78</v>
+        <v>128</v>
       </c>
       <c r="E7" s="13"/>
     </row>
     <row r="8" spans="1:7" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>32</v>
+      <c r="A8" t="s">
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F10" s="15"/>
     </row>
     <row r="11" spans="1:7" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>32</v>
+      <c r="A11" t="s">
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>36</v>
+      <c r="A14" t="s">
+        <v>35</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>36</v>
+      <c r="A15" t="s">
+        <v>35</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E15" s="14"/>
     </row>
     <row r="16" spans="1:7" ht="132" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>37</v>
+      <c r="A16" t="s">
+        <v>36</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
-        <v>37</v>
+      <c r="A17" t="s">
+        <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1514,181 +1495,181 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="181.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>106</v>
+        <v>98</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>110</v>
+        <v>99</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E7" s="21"/>
+        <v>102</v>
+      </c>
+      <c r="E7" s="20"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G9" s="22"/>
+        <v>104</v>
+      </c>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1699,133 +1680,146 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF5D6FA-27AF-4377-9AE3-FE0575D1CE52}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="4" customFormat="1" ht="132" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="132" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>129</v>
+        <v>71</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
       </c>
       <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18"/>
+    </row>
+    <row r="6" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="18"/>
-    </row>
-    <row r="6" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1837,8 +1831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6FF90FC-7D54-4396-BEBF-836B30C262EA}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1846,26 +1840,26 @@
     <col min="1" max="1" width="37.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="33" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="23" style="4" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="17.140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1876,56 +1870,56 @@
     </row>
     <row r="3" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1939,7 +1933,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1956,70 +1950,70 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
         <v>63</v>
-      </c>
-      <c r="E1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -2032,10 +2026,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DAF0C1-5840-4498-93BE-7596EB0B3995}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,118 +2050,101 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="177" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>86</v>
+        <v>132</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" s="4"/>
+        <v>133</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>97</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E10" s="19"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E9" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>